<commit_message>
going to strip down loop for pid calibration
</commit_message>
<xml_diff>
--- a/KiCad documents/HybridChargeControllerBOM.xlsx
+++ b/KiCad documents/HybridChargeControllerBOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,14 +15,14 @@
     <sheet name="HybridChargeController" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HybridChargeController!$A$1:$H$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HybridChargeController!$A$1:$I$28</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="103">
   <si>
     <t>Reference</t>
   </si>
@@ -258,15 +258,6 @@
     <t>6 pin header female</t>
   </si>
   <si>
-    <t>2x8,2x6 pin header male</t>
-  </si>
-  <si>
-    <t>1µ smd</t>
-  </si>
-  <si>
-    <t>0.1µ smd</t>
-  </si>
-  <si>
     <t>P1 P3 P5 P6</t>
   </si>
   <si>
@@ -313,6 +304,33 @@
   </si>
   <si>
     <t>fertig</t>
+  </si>
+  <si>
+    <t>Price 10</t>
+  </si>
+  <si>
+    <t>Price 100</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Pin header</t>
+  </si>
+  <si>
+    <t>2x8, 2x6 male</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>Fuse</t>
+  </si>
+  <si>
+    <t>Screw Terminal</t>
   </si>
 </sst>
 </file>
@@ -860,25 +878,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:J28" totalsRowShown="0">
-  <autoFilter ref="A1:J28">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="y"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:M28" totalsRowShown="0">
+  <autoFilter ref="A1:M28"/>
+  <tableColumns count="13">
     <tableColumn id="1" name="Reference"/>
     <tableColumn id="2" name=" Quantity"/>
     <tableColumn id="3" name=" Value"/>
     <tableColumn id="4" name=" Footprint"/>
     <tableColumn id="5" name="Readable Name"/>
+    <tableColumn id="13" name="Type"/>
     <tableColumn id="6" name="SMD?"/>
     <tableColumn id="7" name="Priority"/>
     <tableColumn id="8" name="available"/>
     <tableColumn id="9" name="Seite"/>
     <tableColumn id="10" name="fertig"/>
+    <tableColumn id="11" name="Price 10"/>
+    <tableColumn id="12" name="Price 100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1181,23 +1196,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="60.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="50.1328125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="50.1328125" customWidth="1"/>
     <col min="5" max="5" width="20.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="20.19921875" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" hidden="1" customWidth="1"/>
+    <col min="9" max="11" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1214,22 +1232,31 @@
         <v>71</v>
       </c>
       <c r="F1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" t="s">
         <v>82</v>
       </c>
-      <c r="G1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" t="s">
-        <v>86</v>
-      </c>
       <c r="I1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" t="s">
         <v>95</v>
       </c>
-      <c r="J1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1243,16 +1270,19 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+        <v>97</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1266,16 +1296,19 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+        <v>99</v>
+      </c>
+      <c r="G3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1292,13 +1325,16 @@
         <v>73</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+        <v>99</v>
+      </c>
+      <c r="G4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1312,16 +1348,19 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+        <v>99</v>
+      </c>
+      <c r="G5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1338,13 +1377,16 @@
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>84</v>
-      </c>
-      <c r="H6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+        <v>100</v>
+      </c>
+      <c r="G6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1361,13 +1403,16 @@
         <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+        <v>100</v>
+      </c>
+      <c r="G7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1384,15 +1429,18 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+        <v>101</v>
+      </c>
+      <c r="G8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -1407,13 +1455,16 @@
         <v>75</v>
       </c>
       <c r="F9" t="s">
-        <v>83</v>
-      </c>
-      <c r="H9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+        <v>102</v>
+      </c>
+      <c r="G9" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1427,16 +1478,19 @@
         <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F10" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+        <v>97</v>
+      </c>
+      <c r="G10" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1453,13 +1507,16 @@
         <v>76</v>
       </c>
       <c r="F11" t="s">
-        <v>83</v>
-      </c>
-      <c r="H11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+        <v>97</v>
+      </c>
+      <c r="G11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1476,13 +1533,16 @@
         <v>77</v>
       </c>
       <c r="F12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+        <v>97</v>
+      </c>
+      <c r="G12" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1498,14 +1558,14 @@
       <c r="E13" t="s">
         <v>33</v>
       </c>
-      <c r="F13" t="s">
-        <v>84</v>
-      </c>
-      <c r="H13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G13" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1521,14 +1581,14 @@
       <c r="E14" t="s">
         <v>36</v>
       </c>
-      <c r="F14" t="s">
-        <v>84</v>
-      </c>
-      <c r="H14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G14" t="s">
+        <v>81</v>
+      </c>
+      <c r="I14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1544,14 +1604,14 @@
       <c r="E15" t="s">
         <v>39</v>
       </c>
-      <c r="F15" t="s">
-        <v>84</v>
-      </c>
-      <c r="H15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G15" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1567,14 +1627,14 @@
       <c r="E16" t="s">
         <v>41</v>
       </c>
-      <c r="F16" t="s">
-        <v>84</v>
-      </c>
-      <c r="H16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1590,14 +1650,14 @@
       <c r="E17" t="s">
         <v>44</v>
       </c>
-      <c r="F17" t="s">
-        <v>84</v>
-      </c>
-      <c r="H17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G17" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -1611,16 +1671,16 @@
         <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F18" t="s">
-        <v>84</v>
-      </c>
-      <c r="H18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+        <v>88</v>
+      </c>
+      <c r="G18" t="s">
+        <v>81</v>
+      </c>
+      <c r="I18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -1636,14 +1696,15 @@
       <c r="E19" s="1">
         <v>100</v>
       </c>
-      <c r="F19" t="s">
-        <v>84</v>
-      </c>
-      <c r="H19" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F19" s="1"/>
+      <c r="G19" t="s">
+        <v>81</v>
+      </c>
+      <c r="I19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -1659,14 +1720,14 @@
       <c r="E20" t="s">
         <v>51</v>
       </c>
-      <c r="F20" t="s">
-        <v>84</v>
-      </c>
-      <c r="H20" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G20" t="s">
+        <v>81</v>
+      </c>
+      <c r="I20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -1682,14 +1743,14 @@
       <c r="E21" t="s">
         <v>53</v>
       </c>
-      <c r="F21" t="s">
-        <v>84</v>
-      </c>
-      <c r="H21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G21" t="s">
+        <v>81</v>
+      </c>
+      <c r="I21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -1705,14 +1766,14 @@
       <c r="E22" t="s">
         <v>55</v>
       </c>
-      <c r="F22" t="s">
-        <v>84</v>
-      </c>
-      <c r="H22" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G22" t="s">
+        <v>81</v>
+      </c>
+      <c r="I22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -1728,14 +1789,14 @@
       <c r="E23" t="s">
         <v>57</v>
       </c>
-      <c r="F23" t="s">
-        <v>84</v>
-      </c>
-      <c r="H23" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G23" t="s">
+        <v>81</v>
+      </c>
+      <c r="I23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>58</v>
       </c>
@@ -1751,14 +1812,14 @@
       <c r="E24" t="s">
         <v>59</v>
       </c>
-      <c r="F24" t="s">
-        <v>84</v>
-      </c>
-      <c r="H24" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G24" t="s">
+        <v>81</v>
+      </c>
+      <c r="I24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -1774,14 +1835,14 @@
       <c r="E25" t="s">
         <v>61</v>
       </c>
-      <c r="F25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G25" t="s">
+        <v>81</v>
+      </c>
+      <c r="I25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -1797,14 +1858,14 @@
       <c r="E26" t="s">
         <v>63</v>
       </c>
-      <c r="F26" t="s">
-        <v>84</v>
-      </c>
-      <c r="H26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G26" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -1820,14 +1881,14 @@
       <c r="E27" t="s">
         <v>66</v>
       </c>
-      <c r="F27" t="s">
-        <v>84</v>
-      </c>
-      <c r="H27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G27" t="s">
+        <v>81</v>
+      </c>
+      <c r="I27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -1843,11 +1904,11 @@
       <c r="E28" t="s">
         <v>69</v>
       </c>
-      <c r="F28" t="s">
-        <v>84</v>
-      </c>
-      <c r="H28" t="s">
-        <v>89</v>
+      <c r="G28" t="s">
+        <v>81</v>
+      </c>
+      <c r="I28" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>